<commit_message>
Updated energy estimates for every country available (with some very crude estimates for missing data)
</commit_message>
<xml_diff>
--- a/ref/validation_workbooks/energy_consumption_init_versus_iea_consumption.xlsx
+++ b/ref/validation_workbooks/energy_consumption_init_versus_iea_consumption.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/validation_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6D3DE3-766D-1740-8392-3D136088EDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C3EE9B-BE69-7C46-9B0B-CEA592B57ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="500" windowWidth="28140" windowHeight="19800" activeTab="3" xr2:uid="{EE3B4993-3866-7E4F-94B3-5CA04524C473}"/>
+    <workbookView xWindow="4160" yWindow="500" windowWidth="23960" windowHeight="19800" activeTab="4" xr2:uid="{EE3B4993-3866-7E4F-94B3-5CA04524C473}"/>
   </bookViews>
   <sheets>
     <sheet name="BRAZIL" sheetId="2" r:id="rId1"/>
     <sheet name="CHILE" sheetId="9" r:id="rId2"/>
     <sheet name="ECUADOR" sheetId="10" r:id="rId3"/>
     <sheet name="MEXICO" sheetId="11" r:id="rId4"/>
-    <sheet name="IEA Energy Efficiency Indicator" sheetId="7" r:id="rId5"/>
-    <sheet name="IEA EEI 2015" sheetId="8" r:id="rId6"/>
-    <sheet name="IEA Summary" sheetId="12" r:id="rId7"/>
+    <sheet name="ALLOCATION_ASSUMPTIONS" sheetId="13" r:id="rId5"/>
+    <sheet name="IEA Energy Efficiency Indicator" sheetId="7" r:id="rId6"/>
+    <sheet name="IEA EEI 2015" sheetId="8" r:id="rId7"/>
+    <sheet name="IEA Summary" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="194">
   <si>
     <t>prodinit_ippu_cement_tonne</t>
   </si>
@@ -468,6 +469,162 @@
   </si>
   <si>
     <t>IEA MANUFACTURING (estimate from IEA Summary Sheet)</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>industries_correspondence = {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'consumpinit_inen_energy_tj_per_tonne_production_electronics' : (0.5, 'Machinery [ISIC 25-28]'), #Electronics is ISIC 26 and 27, so let's say half of 25-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'consumpinit_inen_energy_tj_per_tonne_production_plastic' : (0.5, 'Rubber and plastic [ISIC 22]'), # SEE BELOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'consumpinit_inen_energy_tj_per_tonne_production_chemicals' : (1.0, 'Chemicals and chemical products [ISIC 20-21]'), #OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'consumpinit_inen_energy_tj_per_mmm_gdp_other_product_manufacturing' : (0.7, 'Manufacturing [ISIC 10-18; 20-32]'), #OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'consumpinit_inen_energy_total_pj_agriculture_and_livestock' : (1.0, 'Agriculture, forestry and fishing [ISIC 01-03]'), #OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'consumpinit_inen_energy_tj_per_tonne_production_textiles' : (0.5, 'Textiles and leather [ISIC 13-15]'), #SEE BELOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'consumpinit_inen_energy_tj_per_tonne_production_rubber_and_leather' : (0.5, 'Textiles and leather [ISIC 13-15]'), #+ AND 0.5  'Rubber and plastic [ISIC 22]'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'consumpinit_inen_energy_tj_per_tonne_production_metals' : (1.0, 'Basic metals [ISIC 24]'), #OK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'consumpinit_inen_energy_tj_per_tonne_production_lime_and_carbonite' : (0.05, 'Non-metallic minerals [ISIC 23]'), #FIXED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'consumpinit_inen_energy_tj_per_tonne_production_paper' : (1.0, 'Paper pulp and printing [ISIC 17-18]'),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'consumpinit_inen_energy_tj_per_tonne_production_recycled_wood' : (1.0, 'Wood and wood products [ISIC 16]') #I propose we leave this out entirely, unless we are doing all recyclables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'consumpinit_inen_energy_tj_per_tonne_production_cement' : (0.9, 'Non-metallic minerals [ISIC 23]'), #FIXED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'consumpinit_inen_energy_tj_per_tonne_production_glass' : (0.05, 'Non-metallic minerals [ISIC 23]'), #FIXED</t>
+  </si>
+  <si>
+    <t>PYTHON DICT (FROM MATEO)</t>
+  </si>
+  <si>
+    <t>GLASS EXPECTATION</t>
+  </si>
+  <si>
+    <t>CEMENT EXPECTATION</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.enconman.2007.04.013</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>gj/tonne</t>
+  </si>
+  <si>
+    <t>mmbtu/ton</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>Table 6 totals of 10.5 (flat), 7.4 (container), 16.3 (specialty), 13.1 (flat)</t>
+  </si>
+  <si>
+    <t>gj/mmbtu</t>
+  </si>
+  <si>
+    <t>gj/ton</t>
+  </si>
+  <si>
+    <t>ton/tonne</t>
+  </si>
+  <si>
+    <t>tj/tonne (MEAN)</t>
+  </si>
+  <si>
+    <t>(heat)</t>
+  </si>
+  <si>
+    <t>(elec)</t>
+  </si>
+  <si>
+    <t>kwh/gj</t>
+  </si>
+  <si>
+    <t>kwh/ton</t>
+  </si>
+  <si>
+    <t>tj/tonne</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.esr.2020.100458</t>
+  </si>
+  <si>
+    <t>LIME AND CARBONITE EXPECTATION</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3390/su13073810</t>
+  </si>
+  <si>
+    <t>https://www.osti.gov/servlets/purl/927883 (https://www.osti.gov/biblio/927883)</t>
+  </si>
+  <si>
+    <t>http://dx.doi.org/10.1016/j.energy.2011.02.023</t>
+  </si>
+  <si>
+    <t>In terms of mj/g</t>
+  </si>
+  <si>
+    <t>EXAMPLE CALIBRATION BY COUNTRY WHERE DATA ARE AVAILABLE (MEXICO/BRAZIL)</t>
+  </si>
+  <si>
+    <t>brazil</t>
+  </si>
+  <si>
+    <t>mexico</t>
+  </si>
+  <si>
+    <t>cement</t>
+  </si>
+  <si>
+    <t>glass</t>
+  </si>
+  <si>
+    <t>lime and carbonite</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>INITIAL ENERGY USE (TJ)</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>TOTAL IEA</t>
+  </si>
+  <si>
+    <t>scale_factor</t>
   </si>
 </sst>
 </file>
@@ -478,7 +635,7 @@
     <numFmt numFmtId="164" formatCode="0.00;\-0.00000;0"/>
     <numFmt numFmtId="165" formatCode="0.00_);\(0.00\)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -540,8 +697,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -575,6 +740,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -756,11 +927,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -893,8 +1065,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1210,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A11591-CE4B-574C-A0F9-595E51EFF058}">
   <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32:D34"/>
+    <sheetView zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1820,8 +2013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D96D93-C352-1640-B880-F770081BBE71}">
   <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A14" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3020,8 +3213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD4DA1E-FBFB-644A-8E4F-C9E1F2D0127E}">
   <dimension ref="A1:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3627,6 +3820,638 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8727E570-6B73-A049-A06A-60F4D28F4786}">
+  <dimension ref="A1:L65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="F19" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="K19" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="L19" s="54" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f>AVERAGE(C20,D20)</f>
+        <v>5.875</v>
+      </c>
+      <c r="B20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20">
+        <v>3.85</v>
+      </c>
+      <c r="D20">
+        <v>7.9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>160</v>
+      </c>
+      <c r="J20">
+        <v>1.0550600000000001</v>
+      </c>
+      <c r="K20">
+        <v>1.1023099999999999</v>
+      </c>
+      <c r="L20">
+        <v>277.7777777</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f>AVERAGE(C22,D22)</f>
+        <v>11.850000000000001</v>
+      </c>
+      <c r="B22" t="s">
+        <v>165</v>
+      </c>
+      <c r="C22">
+        <v>7.4</v>
+      </c>
+      <c r="D22">
+        <v>16.3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>180</v>
+      </c>
+      <c r="F22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <f>A22*J20</f>
+        <v>12.502461000000002</v>
+      </c>
+      <c r="B23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <f>A23*K20</f>
+        <v>13.78158778491</v>
+      </c>
+      <c r="B24" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <f>(A24+A20)/2000</f>
+        <v>9.8282938924550006E-3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
+      <c r="K29" s="54"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>3.4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>110</v>
+      </c>
+      <c r="B31" t="s">
+        <v>175</v>
+      </c>
+      <c r="C31" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <f>A31/L20</f>
+        <v>0.39600000011087999</v>
+      </c>
+      <c r="B32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f>A30+A32</f>
+        <v>3.79600000011088</v>
+      </c>
+      <c r="B33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <f>A33*K20</f>
+        <v>4.1843687601222239</v>
+      </c>
+      <c r="B34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <f>A34/1000</f>
+        <v>4.1843687601222238E-3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>169</v>
+      </c>
+      <c r="E37" s="55" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <f>A37*K20/1000</f>
+        <v>4.40924E-3</v>
+      </c>
+      <c r="B38" t="s">
+        <v>176</v>
+      </c>
+      <c r="E38" s="55"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <f>(A35+A38)/2</f>
+        <v>4.2968043800611123E-3</v>
+      </c>
+      <c r="B40" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42" s="54" t="s">
+        <v>178</v>
+      </c>
+      <c r="B42" s="54"/>
+      <c r="C42" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="D42" s="54" t="s">
+        <v>163</v>
+      </c>
+      <c r="E42" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="F42" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="54"/>
+      <c r="K42" s="54"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>4.2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D43">
+        <v>4.3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>181</v>
+      </c>
+      <c r="F43" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <f>A43/1000</f>
+        <v>4.2000000000000006E-3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>184</v>
+      </c>
+      <c r="F49" t="s">
+        <v>185</v>
+      </c>
+      <c r="G49" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="56"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="56"/>
+      <c r="E50">
+        <f>BRAZIL!B3</f>
+        <v>23403862.309999999</v>
+      </c>
+      <c r="F50">
+        <f>MEXICO!B3</f>
+        <v>33397627.309999999</v>
+      </c>
+      <c r="G50">
+        <f>A40</f>
+        <v>4.2968043800611123E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="56"/>
+      <c r="C51" s="56"/>
+      <c r="D51" s="56"/>
+      <c r="E51">
+        <f>BRAZIL!B6</f>
+        <v>296129.28980000003</v>
+      </c>
+      <c r="F51">
+        <f>MEXICO!B6</f>
+        <v>464580.93939999997</v>
+      </c>
+      <c r="G51">
+        <f>A26</f>
+        <v>9.8282938924550006E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="56"/>
+      <c r="C52" s="56"/>
+      <c r="D52" s="56"/>
+      <c r="E52">
+        <f>BRAZIL!B7</f>
+        <v>3150919.4139999999</v>
+      </c>
+      <c r="F52">
+        <f>MEXICO!B7</f>
+        <v>21032.947179999999</v>
+      </c>
+      <c r="G52">
+        <f>A44</f>
+        <v>4.2000000000000006E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" s="53" t="s">
+        <v>190</v>
+      </c>
+      <c r="B53" s="53"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="B54" s="56"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="56"/>
+      <c r="E54">
+        <f>E50*$G50</f>
+        <v>100561.81808395518</v>
+      </c>
+      <c r="F54">
+        <f>F50*$G50</f>
+        <v>143503.07130925663</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="56" t="s">
+        <v>187</v>
+      </c>
+      <c r="B55" s="56"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55">
+        <f t="shared" ref="E55:F55" si="0">E51*$G51</f>
+        <v>2910.4456903183773</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>4566.0380092560263</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" s="56" t="s">
+        <v>188</v>
+      </c>
+      <c r="B56" s="56"/>
+      <c r="C56" s="56"/>
+      <c r="D56" s="56"/>
+      <c r="E56">
+        <f t="shared" ref="E56:F56" si="1">E52*$G52</f>
+        <v>13233.861538800002</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="1"/>
+        <v>88.338378156000005</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="B57" s="53"/>
+      <c r="C57" s="53"/>
+      <c r="D57" s="53"/>
+      <c r="E57">
+        <f>SUM(E54:E56)/1000</f>
+        <v>116.70612531307356</v>
+      </c>
+      <c r="F57">
+        <f>SUM(F54:F56)/1000</f>
+        <v>148.15744769666867</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="56" t="s">
+        <v>192</v>
+      </c>
+      <c r="B59" s="56"/>
+      <c r="C59" s="56"/>
+      <c r="D59" s="56"/>
+      <c r="E59">
+        <f>BRAZIL!D25</f>
+        <v>378.81</v>
+      </c>
+      <c r="F59">
+        <f>MEXICO!D25</f>
+        <v>218.78</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="56" t="s">
+        <v>193</v>
+      </c>
+      <c r="B60" s="56"/>
+      <c r="C60" s="56"/>
+      <c r="D60" s="56"/>
+      <c r="E60">
+        <f>E59/E57</f>
+        <v>3.2458450572650901</v>
+      </c>
+      <c r="F60">
+        <f>F59/F57</f>
+        <v>1.4766723063961049</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" s="57"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="57"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" s="58"/>
+      <c r="B62" s="58"/>
+      <c r="C62" s="58"/>
+      <c r="D62" s="58"/>
+      <c r="E62" s="61" t="str">
+        <f>E49</f>
+        <v>brazil</v>
+      </c>
+      <c r="F62" s="61" t="str">
+        <f>F49</f>
+        <v>mexico</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" s="60"/>
+      <c r="C63" s="60"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="59">
+        <f>$G50*E$60</f>
+        <v>1.3946761259056351E-2</v>
+      </c>
+      <c r="F63" s="59">
+        <f>$G50*F$60</f>
+        <v>6.3449720340377283E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" s="60"/>
+      <c r="C64" s="60"/>
+      <c r="D64" s="60"/>
+      <c r="E64" s="59">
+        <f>$G51*E$60</f>
+        <v>3.1901119152173738E-2</v>
+      </c>
+      <c r="F64" s="59">
+        <f>$G51*F$60</f>
+        <v>1.4513169410110277E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B65" s="60"/>
+      <c r="C65" s="60"/>
+      <c r="D65" s="60"/>
+      <c r="E65" s="59">
+        <f>$G52*E$60</f>
+        <v>1.3632549240513381E-2</v>
+      </c>
+      <c r="F65" s="59">
+        <f>$G52*F$60</f>
+        <v>6.2020236868636416E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A57:D57"/>
+    <mergeCell ref="A53:F53"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="A56:D56"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E37" r:id="rId1" xr:uid="{EBC76CDC-BF99-444B-A86B-9D5AC2231412}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF156F7-DDA6-0E44-875B-739D60BEC496}">
   <dimension ref="A1:X61"/>
   <sheetViews>
@@ -8161,12 +8986,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD5630A-52D1-5C4C-9BA6-20F6E7F00A3C}">
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8587,7 +9412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED32E5F2-EDC7-1848-B301-8B79B7F979E3}">
   <dimension ref="A1:Q14"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated transformations build for energy and added and reorganized transformations
</commit_message>
<xml_diff>
--- a/ref/validation_workbooks/energy_consumption_init_versus_iea_consumption.xlsx
+++ b/ref/validation_workbooks/energy_consumption_init_versus_iea_consumption.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/validation_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C3EE9B-BE69-7C46-9B0B-CEA592B57ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA4C04D-4C43-5044-9756-3EC9E3BC8921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="500" windowWidth="23960" windowHeight="19800" activeTab="4" xr2:uid="{EE3B4993-3866-7E4F-94B3-5CA04524C473}"/>
+    <workbookView xWindow="12580" yWindow="1360" windowWidth="23960" windowHeight="19800" activeTab="4" xr2:uid="{EE3B4993-3866-7E4F-94B3-5CA04524C473}"/>
   </bookViews>
   <sheets>
     <sheet name="BRAZIL" sheetId="2" r:id="rId1"/>
@@ -1079,11 +1079,11 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3824,7 +3824,7 @@
   <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4371,22 +4371,22 @@
       <c r="B62" s="58"/>
       <c r="C62" s="58"/>
       <c r="D62" s="58"/>
-      <c r="E62" s="61" t="str">
+      <c r="E62" s="60" t="str">
         <f>E49</f>
         <v>brazil</v>
       </c>
-      <c r="F62" s="61" t="str">
+      <c r="F62" s="60" t="str">
         <f>F49</f>
         <v>mexico</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="60" t="s">
+      <c r="A63" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B63" s="60"/>
-      <c r="C63" s="60"/>
-      <c r="D63" s="60"/>
+      <c r="B63" s="61"/>
+      <c r="C63" s="61"/>
+      <c r="D63" s="61"/>
       <c r="E63" s="59">
         <f>$G50*E$60</f>
         <v>1.3946761259056351E-2</v>
@@ -4397,12 +4397,12 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="60" t="s">
+      <c r="A64" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="B64" s="60"/>
-      <c r="C64" s="60"/>
-      <c r="D64" s="60"/>
+      <c r="B64" s="61"/>
+      <c r="C64" s="61"/>
+      <c r="D64" s="61"/>
       <c r="E64" s="59">
         <f>$G51*E$60</f>
         <v>3.1901119152173738E-2</v>
@@ -4413,12 +4413,12 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="60" t="s">
+      <c r="A65" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="B65" s="60"/>
-      <c r="C65" s="60"/>
-      <c r="D65" s="60"/>
+      <c r="B65" s="61"/>
+      <c r="C65" s="61"/>
+      <c r="D65" s="61"/>
       <c r="E65" s="59">
         <f>$G52*E$60</f>
         <v>1.3632549240513381E-2</v>

</xml_diff>